<commit_message>
+ fixed some case-sensitivity issues reported by Christopher Nitta, UC Davis, who was running on Linux & OS-X + replaced call to GaussElim in ElastoDyn with call to LAPACK routines. + added option to print mesh name in DrawMesh.m (called from FASTInputMeshes.m) + added DWM in compile scripts + added a couple of missing spaces in CompilingInstructions_FASTv8.docx + renamed InflowWind's registry files to correspond to Andy P's reorg of InflowWind
git-svn-id: https://windsvn2.nrel.gov/FAST/branches/BJonkman/Utilities/SimulationToolbox@776 10acb478-4768-415a-8850-bacdb5912d4d
</commit_message>
<xml_diff>
--- a/ConvertFASTversions/TemplateFiles/v8.00.x/OutListParameters.xlsx
+++ b/ConvertFASTversions/TemplateFiles/v8.00.x/OutListParameters.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21390" windowHeight="9570" activeTab="7"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="21390" windowHeight="9570" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="8" r:id="rId1"/>
@@ -22402,7 +22402,7 @@
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -22820,7 +22820,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -37571,7 +37573,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>